<commit_message>
Test data is added
The added files was updated according to recommendations
</commit_message>
<xml_diff>
--- a/Lesson3/Test Execution Report_Calc_Iryna_Lukovets.xlsx
+++ b/Lesson3/Test Execution Report_Calc_Iryna_Lukovets.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="159">
   <si>
     <t>Traceability matrix</t>
   </si>
@@ -156,13 +156,7 @@
     <t>3. Check the presence of the buttons "sqrt", "%", "1/x", "lg"</t>
   </si>
   <si>
-    <t>The button "lg" is absent, all other bottons are present</t>
-  </si>
-  <si>
     <t>1.3. Check the possibility to enter data and make calculations using the calculator buttons</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1. Enter each of digits </t>
   </si>
   <si>
     <t>1.1. Check the presence of the field for entering data/result output field</t>
@@ -503,21 +497,6 @@
   </si>
   <si>
     <t xml:space="preserve">4. </t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">The button "7" can't be clicked, it is impossible to enter the digit "7" using the calculator buttons. </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>All other buttons work and it is possible to enter data and get result using the calculator buttons</t>
-    </r>
   </si>
   <si>
     <t>It is impossible to get result of any calculation using the keyboard because all characters include "+", "-", "=" etc. are written in the field by the line</t>
@@ -574,6 +553,33 @@
   </si>
   <si>
     <t>It is impossible to calculate the decimal logarithm because the button "lg" is absent</t>
+  </si>
+  <si>
+    <t>The button "lg" is absent, all other buttons are present</t>
+  </si>
+  <si>
+    <t>1. Enter each of digits and symbols</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">The button "7" can't be clicked, it is impossible to enter the digit "7" using the calculator buttons. If press"+/-" before pressing any digit the app fails to respond.  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>All other buttons work and it is possible to enter data and get result using the calculator buttons</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">10. </t>
+  </si>
+  <si>
+    <t>If press"+/-" before pressing any digit the app fails to respond.</t>
   </si>
 </sst>
 </file>
@@ -1093,6 +1099,13 @@
     <xf numFmtId="49" fontId="9" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1" shrinkToFit="1"/>
     </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="15" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="20" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1" shrinkToFit="1"/>
+    </xf>
     <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
@@ -1123,12 +1136,10 @@
     <xf numFmtId="49" fontId="1" fillId="0" borderId="21" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="49" fontId="6" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1137,13 +1148,8 @@
     <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="15" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="20" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1" shrinkToFit="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -1427,7 +1433,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y23"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
+    <sheetView topLeftCell="C13" workbookViewId="0">
       <selection activeCell="E6" sqref="E6:E19"/>
     </sheetView>
   </sheetViews>
@@ -1496,11 +1502,11 @@
     <row r="3" spans="1:25" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
-      <c r="C3" s="28" t="s">
+      <c r="C3" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="29"/>
-      <c r="E3" s="30"/>
+      <c r="D3" s="32"/>
+      <c r="E3" s="33"/>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
@@ -1525,11 +1531,11 @@
     <row r="4" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
-      <c r="C4" s="31" t="s">
+      <c r="C4" s="34" t="s">
         <v>16</v>
       </c>
-      <c r="D4" s="32"/>
-      <c r="E4" s="33"/>
+      <c r="D4" s="35"/>
+      <c r="E4" s="36"/>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
@@ -1585,14 +1591,14 @@
     <row r="6" spans="1:25" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
-      <c r="C6" s="34" t="s">
+      <c r="C6" s="37" t="s">
         <v>20</v>
       </c>
       <c r="D6" s="5" t="s">
         <v>9</v>
       </c>
       <c r="E6" s="18" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
@@ -1618,7 +1624,7 @@
     <row r="7" spans="1:25" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
-      <c r="C7" s="35"/>
+      <c r="C7" s="38"/>
       <c r="D7" s="5" t="s">
         <v>10</v>
       </c>
@@ -1649,11 +1655,11 @@
     <row r="8" spans="1:25" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="16"/>
       <c r="B8" s="16"/>
-      <c r="C8" s="35"/>
+      <c r="C8" s="38"/>
       <c r="D8" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="E8" s="44" t="s">
+      <c r="E8" s="28" t="s">
         <v>23</v>
       </c>
       <c r="F8" s="16"/>
@@ -1680,12 +1686,12 @@
     <row r="9" spans="1:25" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="16"/>
       <c r="B9" s="16"/>
-      <c r="C9" s="35"/>
+      <c r="C9" s="38"/>
       <c r="D9" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="E9" s="44" t="s">
-        <v>46</v>
+      <c r="E9" s="28" t="s">
+        <v>44</v>
       </c>
       <c r="F9" s="16"/>
       <c r="G9" s="16"/>
@@ -1711,11 +1717,11 @@
     <row r="10" spans="1:25" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="16"/>
       <c r="B10" s="16"/>
-      <c r="C10" s="35"/>
+      <c r="C10" s="38"/>
       <c r="D10" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="E10" s="44" t="s">
+      <c r="E10" s="28" t="s">
         <v>22</v>
       </c>
       <c r="F10" s="16"/>
@@ -1742,14 +1748,14 @@
     <row r="11" spans="1:25" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
-      <c r="C11" s="36" t="s">
+      <c r="C11" s="39" t="s">
         <v>17</v>
       </c>
       <c r="D11" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="E11" s="46" t="s">
-        <v>58</v>
+      <c r="E11" s="30" t="s">
+        <v>56</v>
       </c>
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
@@ -1775,12 +1781,12 @@
     <row r="12" spans="1:25" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
-      <c r="C12" s="35"/>
+      <c r="C12" s="38"/>
       <c r="D12" s="5" t="s">
         <v>13</v>
       </c>
       <c r="E12" s="18" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
@@ -1806,12 +1812,12 @@
     <row r="13" spans="1:25" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
-      <c r="C13" s="35"/>
+      <c r="C13" s="38"/>
       <c r="D13" s="5" t="s">
         <v>14</v>
       </c>
       <c r="E13" s="18" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
@@ -1837,12 +1843,12 @@
     <row r="14" spans="1:25" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="25"/>
       <c r="B14" s="25"/>
-      <c r="C14" s="35"/>
+      <c r="C14" s="38"/>
       <c r="D14" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="E14" s="44" t="s">
-        <v>87</v>
+      <c r="E14" s="28" t="s">
+        <v>85</v>
       </c>
       <c r="F14" s="25"/>
       <c r="G14" s="25"/>
@@ -1868,12 +1874,12 @@
     <row r="15" spans="1:25" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="25"/>
       <c r="B15" s="25"/>
-      <c r="C15" s="35"/>
+      <c r="C15" s="38"/>
       <c r="D15" s="6" t="s">
-        <v>94</v>
-      </c>
-      <c r="E15" s="44" t="s">
-        <v>95</v>
+        <v>92</v>
+      </c>
+      <c r="E15" s="28" t="s">
+        <v>93</v>
       </c>
       <c r="F15" s="25"/>
       <c r="G15" s="25"/>
@@ -1899,12 +1905,12 @@
     <row r="16" spans="1:25" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="25"/>
       <c r="B16" s="25"/>
-      <c r="C16" s="35"/>
+      <c r="C16" s="38"/>
       <c r="D16" s="6" t="s">
-        <v>105</v>
-      </c>
-      <c r="E16" s="44" t="s">
-        <v>106</v>
+        <v>103</v>
+      </c>
+      <c r="E16" s="28" t="s">
+        <v>104</v>
       </c>
       <c r="F16" s="25"/>
       <c r="G16" s="25"/>
@@ -1930,12 +1936,12 @@
     <row r="17" spans="1:25" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="25"/>
       <c r="B17" s="25"/>
-      <c r="C17" s="35"/>
+      <c r="C17" s="38"/>
       <c r="D17" s="6" t="s">
-        <v>113</v>
-      </c>
-      <c r="E17" s="44" t="s">
-        <v>119</v>
+        <v>111</v>
+      </c>
+      <c r="E17" s="28" t="s">
+        <v>117</v>
       </c>
       <c r="F17" s="25"/>
       <c r="G17" s="25"/>
@@ -1961,12 +1967,12 @@
     <row r="18" spans="1:25" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="25"/>
       <c r="B18" s="25"/>
-      <c r="C18" s="35"/>
+      <c r="C18" s="38"/>
       <c r="D18" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="E18" s="28" t="s">
         <v>118</v>
-      </c>
-      <c r="E18" s="44" t="s">
-        <v>120</v>
       </c>
       <c r="F18" s="25"/>
       <c r="G18" s="25"/>
@@ -1992,12 +1998,12 @@
     <row r="19" spans="1:25" ht="77.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
-      <c r="C19" s="37"/>
+      <c r="C19" s="40"/>
       <c r="D19" s="21" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="E19" s="22" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="F19" s="1"/>
       <c r="G19" s="1"/>
@@ -2144,8 +2150,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T151"/>
   <sheetViews>
-    <sheetView topLeftCell="A142" workbookViewId="0">
-      <selection activeCell="B81" sqref="B81"/>
+    <sheetView topLeftCell="A79" workbookViewId="0">
+      <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2155,26 +2161,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A1" s="42" t="s">
+      <c r="A1" s="43" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="42"/>
-      <c r="C1" s="42"/>
-      <c r="D1" s="42"/>
-      <c r="E1" s="42"/>
-      <c r="F1" s="42"/>
-      <c r="G1" s="42"/>
-      <c r="H1" s="42"/>
-      <c r="I1" s="42"/>
-      <c r="J1" s="42"/>
-      <c r="K1" s="42"/>
-      <c r="L1" s="42"/>
-      <c r="M1" s="42"/>
-      <c r="N1" s="42"/>
-      <c r="O1" s="42"/>
-      <c r="P1" s="42"/>
-      <c r="Q1" s="42"/>
-      <c r="R1" s="42"/>
+      <c r="B1" s="43"/>
+      <c r="C1" s="43"/>
+      <c r="D1" s="43"/>
+      <c r="E1" s="43"/>
+      <c r="F1" s="43"/>
+      <c r="G1" s="43"/>
+      <c r="H1" s="43"/>
+      <c r="I1" s="43"/>
+      <c r="J1" s="43"/>
+      <c r="K1" s="43"/>
+      <c r="L1" s="43"/>
+      <c r="M1" s="43"/>
+      <c r="N1" s="43"/>
+      <c r="O1" s="43"/>
+      <c r="P1" s="43"/>
+      <c r="Q1" s="43"/>
+      <c r="R1" s="43"/>
       <c r="S1" s="1"/>
       <c r="T1" s="1"/>
     </row>
@@ -2296,7 +2302,7 @@
     </row>
     <row r="7" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="41" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B7" s="41"/>
       <c r="C7" s="41"/>
@@ -2319,11 +2325,11 @@
       <c r="T7" s="1"/>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A8" s="43" t="s">
+      <c r="A8" s="44" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="43"/>
-      <c r="C8" s="43"/>
+      <c r="B8" s="44"/>
+      <c r="C8" s="44"/>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
@@ -2343,18 +2349,18 @@
       <c r="T8" s="1"/>
     </row>
     <row r="9" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="40" t="s">
-        <v>37</v>
-      </c>
-      <c r="B9" s="40"/>
-      <c r="C9" s="40"/>
-      <c r="D9" s="40"/>
-      <c r="E9" s="40"/>
-      <c r="F9" s="40"/>
-      <c r="G9" s="40"/>
-      <c r="H9" s="40"/>
-      <c r="I9" s="40"/>
-      <c r="J9" s="40"/>
+      <c r="A9" s="42" t="s">
+        <v>35</v>
+      </c>
+      <c r="B9" s="42"/>
+      <c r="C9" s="42"/>
+      <c r="D9" s="42"/>
+      <c r="E9" s="42"/>
+      <c r="F9" s="42"/>
+      <c r="G9" s="42"/>
+      <c r="H9" s="42"/>
+      <c r="I9" s="42"/>
+      <c r="J9" s="42"/>
       <c r="K9" s="1"/>
       <c r="L9" s="1"/>
       <c r="M9" s="1"/>
@@ -2367,18 +2373,18 @@
       <c r="T9" s="1"/>
     </row>
     <row r="10" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="40" t="s">
-        <v>38</v>
-      </c>
-      <c r="B10" s="40"/>
-      <c r="C10" s="40"/>
-      <c r="D10" s="40"/>
-      <c r="E10" s="40"/>
-      <c r="F10" s="40"/>
-      <c r="G10" s="40"/>
-      <c r="H10" s="40"/>
-      <c r="I10" s="40"/>
-      <c r="J10" s="40"/>
+      <c r="A10" s="42" t="s">
+        <v>36</v>
+      </c>
+      <c r="B10" s="42"/>
+      <c r="C10" s="42"/>
+      <c r="D10" s="42"/>
+      <c r="E10" s="42"/>
+      <c r="F10" s="42"/>
+      <c r="G10" s="42"/>
+      <c r="H10" s="42"/>
+      <c r="I10" s="42"/>
+      <c r="J10" s="42"/>
       <c r="K10" s="1"/>
       <c r="L10" s="1"/>
       <c r="M10" s="1"/>
@@ -2442,10 +2448,10 @@
     </row>
     <row r="13" spans="1:20" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="12" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B13" s="13" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
@@ -2537,18 +2543,18 @@
       <c r="T16" s="1"/>
     </row>
     <row r="17" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="40" t="s">
+      <c r="A17" s="42" t="s">
         <v>28</v>
       </c>
-      <c r="B17" s="40"/>
-      <c r="C17" s="40"/>
-      <c r="D17" s="40"/>
-      <c r="E17" s="40"/>
-      <c r="F17" s="40"/>
-      <c r="G17" s="40"/>
-      <c r="H17" s="40"/>
-      <c r="I17" s="40"/>
-      <c r="J17" s="40"/>
+      <c r="B17" s="42"/>
+      <c r="C17" s="42"/>
+      <c r="D17" s="42"/>
+      <c r="E17" s="42"/>
+      <c r="F17" s="42"/>
+      <c r="G17" s="42"/>
+      <c r="H17" s="42"/>
+      <c r="I17" s="42"/>
+      <c r="J17" s="42"/>
       <c r="K17" s="1"/>
       <c r="L17" s="1"/>
       <c r="M17" s="1"/>
@@ -2561,18 +2567,18 @@
       <c r="T17" s="1"/>
     </row>
     <row r="18" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A18" s="40" t="s">
+      <c r="A18" s="42" t="s">
         <v>29</v>
       </c>
-      <c r="B18" s="40"/>
-      <c r="C18" s="40"/>
-      <c r="D18" s="40"/>
-      <c r="E18" s="40"/>
-      <c r="F18" s="40"/>
-      <c r="G18" s="40"/>
-      <c r="H18" s="40"/>
-      <c r="I18" s="40"/>
-      <c r="J18" s="40"/>
+      <c r="B18" s="42"/>
+      <c r="C18" s="42"/>
+      <c r="D18" s="42"/>
+      <c r="E18" s="42"/>
+      <c r="F18" s="42"/>
+      <c r="G18" s="42"/>
+      <c r="H18" s="42"/>
+      <c r="I18" s="42"/>
+      <c r="J18" s="42"/>
       <c r="K18" s="1"/>
       <c r="L18" s="1"/>
       <c r="M18" s="1"/>
@@ -2585,18 +2591,18 @@
       <c r="T18" s="1"/>
     </row>
     <row r="19" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A19" s="40" t="s">
+      <c r="A19" s="42" t="s">
         <v>31</v>
       </c>
-      <c r="B19" s="40"/>
-      <c r="C19" s="40"/>
-      <c r="D19" s="40"/>
-      <c r="E19" s="40"/>
-      <c r="F19" s="40"/>
-      <c r="G19" s="40"/>
-      <c r="H19" s="40"/>
-      <c r="I19" s="40"/>
-      <c r="J19" s="40"/>
+      <c r="B19" s="42"/>
+      <c r="C19" s="42"/>
+      <c r="D19" s="42"/>
+      <c r="E19" s="42"/>
+      <c r="F19" s="42"/>
+      <c r="G19" s="42"/>
+      <c r="H19" s="42"/>
+      <c r="I19" s="42"/>
+      <c r="J19" s="42"/>
       <c r="K19" s="16"/>
       <c r="L19" s="16"/>
       <c r="M19" s="16"/>
@@ -2663,7 +2669,7 @@
         <v>30</v>
       </c>
       <c r="B22" s="27" t="s">
-        <v>32</v>
+        <v>154</v>
       </c>
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
@@ -2708,7 +2714,7 @@
     </row>
     <row r="24" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A24" s="41" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B24" s="41"/>
       <c r="C24" s="41"/>
@@ -2756,7 +2762,7 @@
     </row>
     <row r="26" spans="1:20" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="24" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B26" s="8"/>
       <c r="C26" s="8"/>
@@ -2803,18 +2809,18 @@
       <c r="T27" s="1"/>
     </row>
     <row r="28" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="40" t="s">
-        <v>34</v>
-      </c>
-      <c r="B28" s="40"/>
-      <c r="C28" s="40"/>
-      <c r="D28" s="40"/>
-      <c r="E28" s="40"/>
-      <c r="F28" s="40"/>
-      <c r="G28" s="40"/>
-      <c r="H28" s="40"/>
-      <c r="I28" s="40"/>
-      <c r="J28" s="40"/>
+      <c r="A28" s="42" t="s">
+        <v>155</v>
+      </c>
+      <c r="B28" s="42"/>
+      <c r="C28" s="42"/>
+      <c r="D28" s="42"/>
+      <c r="E28" s="42"/>
+      <c r="F28" s="42"/>
+      <c r="G28" s="42"/>
+      <c r="H28" s="42"/>
+      <c r="I28" s="42"/>
+      <c r="J28" s="42"/>
       <c r="K28" s="1"/>
       <c r="L28" s="1"/>
       <c r="M28" s="1"/>
@@ -2827,18 +2833,18 @@
       <c r="T28" s="1"/>
     </row>
     <row r="29" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="40" t="s">
-        <v>42</v>
-      </c>
-      <c r="B29" s="40"/>
-      <c r="C29" s="40"/>
-      <c r="D29" s="40"/>
-      <c r="E29" s="40"/>
-      <c r="F29" s="40"/>
-      <c r="G29" s="40"/>
-      <c r="H29" s="40"/>
-      <c r="I29" s="40"/>
-      <c r="J29" s="40"/>
+      <c r="A29" s="42" t="s">
+        <v>40</v>
+      </c>
+      <c r="B29" s="42"/>
+      <c r="C29" s="42"/>
+      <c r="D29" s="42"/>
+      <c r="E29" s="42"/>
+      <c r="F29" s="42"/>
+      <c r="G29" s="42"/>
+      <c r="H29" s="42"/>
+      <c r="I29" s="42"/>
+      <c r="J29" s="42"/>
       <c r="K29" s="16"/>
       <c r="L29" s="16"/>
       <c r="M29" s="16"/>
@@ -2851,18 +2857,18 @@
       <c r="T29" s="16"/>
     </row>
     <row r="30" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A30" s="40" t="s">
-        <v>43</v>
-      </c>
-      <c r="B30" s="40"/>
-      <c r="C30" s="40"/>
-      <c r="D30" s="40"/>
-      <c r="E30" s="40"/>
-      <c r="F30" s="40"/>
-      <c r="G30" s="40"/>
-      <c r="H30" s="40"/>
-      <c r="I30" s="40"/>
-      <c r="J30" s="40"/>
+      <c r="A30" s="42" t="s">
+        <v>41</v>
+      </c>
+      <c r="B30" s="42"/>
+      <c r="C30" s="42"/>
+      <c r="D30" s="42"/>
+      <c r="E30" s="42"/>
+      <c r="F30" s="42"/>
+      <c r="G30" s="42"/>
+      <c r="H30" s="42"/>
+      <c r="I30" s="42"/>
+      <c r="J30" s="42"/>
       <c r="K30" s="1"/>
       <c r="L30" s="1"/>
       <c r="M30" s="1"/>
@@ -2875,18 +2881,18 @@
       <c r="T30" s="1"/>
     </row>
     <row r="31" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A31" s="40" t="s">
-        <v>40</v>
-      </c>
-      <c r="B31" s="40"/>
-      <c r="C31" s="40"/>
-      <c r="D31" s="40"/>
-      <c r="E31" s="40"/>
-      <c r="F31" s="40"/>
-      <c r="G31" s="40"/>
-      <c r="H31" s="40"/>
-      <c r="I31" s="40"/>
-      <c r="J31" s="40"/>
+      <c r="A31" s="42" t="s">
+        <v>38</v>
+      </c>
+      <c r="B31" s="42"/>
+      <c r="C31" s="42"/>
+      <c r="D31" s="42"/>
+      <c r="E31" s="42"/>
+      <c r="F31" s="42"/>
+      <c r="G31" s="42"/>
+      <c r="H31" s="42"/>
+      <c r="I31" s="42"/>
+      <c r="J31" s="42"/>
       <c r="K31" s="16"/>
       <c r="L31" s="16"/>
       <c r="M31" s="16"/>
@@ -2948,12 +2954,12 @@
       <c r="S33" s="1"/>
       <c r="T33" s="1"/>
     </row>
-    <row r="34" spans="1:20" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:20" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="12" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B34" s="27" t="s">
-        <v>144</v>
+        <v>156</v>
       </c>
       <c r="C34" s="1"/>
       <c r="D34" s="1"/>
@@ -2998,7 +3004,7 @@
     </row>
     <row r="36" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A36" s="41" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B36" s="41"/>
       <c r="C36" s="41"/>
@@ -3046,7 +3052,7 @@
     </row>
     <row r="38" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
@@ -3093,18 +3099,18 @@
       <c r="T39" s="1"/>
     </row>
     <row r="40" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A40" s="40" t="s">
-        <v>48</v>
-      </c>
-      <c r="B40" s="40"/>
-      <c r="C40" s="40"/>
-      <c r="D40" s="40"/>
-      <c r="E40" s="40"/>
-      <c r="F40" s="40"/>
-      <c r="G40" s="40"/>
-      <c r="H40" s="40"/>
-      <c r="I40" s="40"/>
-      <c r="J40" s="40"/>
+      <c r="A40" s="42" t="s">
+        <v>46</v>
+      </c>
+      <c r="B40" s="42"/>
+      <c r="C40" s="42"/>
+      <c r="D40" s="42"/>
+      <c r="E40" s="42"/>
+      <c r="F40" s="42"/>
+      <c r="G40" s="42"/>
+      <c r="H40" s="42"/>
+      <c r="I40" s="42"/>
+      <c r="J40" s="42"/>
       <c r="K40" s="1"/>
       <c r="L40" s="1"/>
       <c r="M40" s="1"/>
@@ -3117,18 +3123,18 @@
       <c r="T40" s="1"/>
     </row>
     <row r="41" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A41" s="40" t="s">
-        <v>54</v>
-      </c>
-      <c r="B41" s="40"/>
-      <c r="C41" s="40"/>
-      <c r="D41" s="40"/>
-      <c r="E41" s="40"/>
-      <c r="F41" s="40"/>
-      <c r="G41" s="40"/>
-      <c r="H41" s="40"/>
-      <c r="I41" s="40"/>
-      <c r="J41" s="40"/>
+      <c r="A41" s="42" t="s">
+        <v>52</v>
+      </c>
+      <c r="B41" s="42"/>
+      <c r="C41" s="42"/>
+      <c r="D41" s="42"/>
+      <c r="E41" s="42"/>
+      <c r="F41" s="42"/>
+      <c r="G41" s="42"/>
+      <c r="H41" s="42"/>
+      <c r="I41" s="42"/>
+      <c r="J41" s="42"/>
       <c r="K41" s="16"/>
       <c r="L41" s="16"/>
       <c r="M41" s="16"/>
@@ -3141,18 +3147,18 @@
       <c r="T41" s="16"/>
     </row>
     <row r="42" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A42" s="40" t="s">
-        <v>55</v>
-      </c>
-      <c r="B42" s="40"/>
-      <c r="C42" s="40"/>
-      <c r="D42" s="40"/>
-      <c r="E42" s="40"/>
-      <c r="F42" s="40"/>
-      <c r="G42" s="40"/>
-      <c r="H42" s="40"/>
-      <c r="I42" s="40"/>
-      <c r="J42" s="40"/>
+      <c r="A42" s="42" t="s">
+        <v>53</v>
+      </c>
+      <c r="B42" s="42"/>
+      <c r="C42" s="42"/>
+      <c r="D42" s="42"/>
+      <c r="E42" s="42"/>
+      <c r="F42" s="42"/>
+      <c r="G42" s="42"/>
+      <c r="H42" s="42"/>
+      <c r="I42" s="42"/>
+      <c r="J42" s="42"/>
       <c r="K42" s="16"/>
       <c r="L42" s="16"/>
       <c r="M42" s="16"/>
@@ -3165,18 +3171,18 @@
       <c r="T42" s="16"/>
     </row>
     <row r="43" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A43" s="40" t="s">
-        <v>63</v>
-      </c>
-      <c r="B43" s="40"/>
-      <c r="C43" s="40"/>
-      <c r="D43" s="40"/>
-      <c r="E43" s="40"/>
-      <c r="F43" s="40"/>
-      <c r="G43" s="40"/>
-      <c r="H43" s="40"/>
-      <c r="I43" s="40"/>
-      <c r="J43" s="40"/>
+      <c r="A43" s="42" t="s">
+        <v>61</v>
+      </c>
+      <c r="B43" s="42"/>
+      <c r="C43" s="42"/>
+      <c r="D43" s="42"/>
+      <c r="E43" s="42"/>
+      <c r="F43" s="42"/>
+      <c r="G43" s="42"/>
+      <c r="H43" s="42"/>
+      <c r="I43" s="42"/>
+      <c r="J43" s="42"/>
       <c r="K43" s="1"/>
       <c r="L43" s="1"/>
       <c r="M43" s="1"/>
@@ -3240,10 +3246,10 @@
     </row>
     <row r="46" spans="1:20" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="12" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B46" s="27" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C46" s="1"/>
       <c r="D46" s="1"/>
@@ -3288,7 +3294,7 @@
     </row>
     <row r="48" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A48" s="41" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B48" s="41"/>
       <c r="C48" s="41"/>
@@ -3336,7 +3342,7 @@
     </row>
     <row r="50" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B50" s="1"/>
       <c r="C50" s="1"/>
@@ -3360,7 +3366,7 @@
     </row>
     <row r="51" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A51" s="16" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B51" s="16"/>
       <c r="C51" s="16"/>
@@ -3407,18 +3413,18 @@
       <c r="T52" s="1"/>
     </row>
     <row r="53" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="40" t="s">
-        <v>48</v>
-      </c>
-      <c r="B53" s="40"/>
-      <c r="C53" s="40"/>
-      <c r="D53" s="40"/>
-      <c r="E53" s="40"/>
-      <c r="F53" s="40"/>
-      <c r="G53" s="40"/>
-      <c r="H53" s="40"/>
-      <c r="I53" s="40"/>
-      <c r="J53" s="40"/>
+      <c r="A53" s="42" t="s">
+        <v>46</v>
+      </c>
+      <c r="B53" s="42"/>
+      <c r="C53" s="42"/>
+      <c r="D53" s="42"/>
+      <c r="E53" s="42"/>
+      <c r="F53" s="42"/>
+      <c r="G53" s="42"/>
+      <c r="H53" s="42"/>
+      <c r="I53" s="42"/>
+      <c r="J53" s="42"/>
       <c r="K53" s="1"/>
       <c r="L53" s="1"/>
       <c r="M53" s="1"/>
@@ -3431,18 +3437,18 @@
       <c r="T53" s="1"/>
     </row>
     <row r="54" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="40" t="s">
-        <v>56</v>
-      </c>
-      <c r="B54" s="40"/>
-      <c r="C54" s="40"/>
-      <c r="D54" s="40"/>
-      <c r="E54" s="40"/>
-      <c r="F54" s="40"/>
-      <c r="G54" s="40"/>
-      <c r="H54" s="40"/>
-      <c r="I54" s="40"/>
-      <c r="J54" s="40"/>
+      <c r="A54" s="42" t="s">
+        <v>54</v>
+      </c>
+      <c r="B54" s="42"/>
+      <c r="C54" s="42"/>
+      <c r="D54" s="42"/>
+      <c r="E54" s="42"/>
+      <c r="F54" s="42"/>
+      <c r="G54" s="42"/>
+      <c r="H54" s="42"/>
+      <c r="I54" s="42"/>
+      <c r="J54" s="42"/>
       <c r="K54" s="1"/>
       <c r="L54" s="1"/>
       <c r="M54" s="1"/>
@@ -3455,18 +3461,18 @@
       <c r="T54" s="1"/>
     </row>
     <row r="55" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A55" s="40" t="s">
-        <v>57</v>
-      </c>
-      <c r="B55" s="40"/>
-      <c r="C55" s="40"/>
-      <c r="D55" s="40"/>
-      <c r="E55" s="40"/>
-      <c r="F55" s="40"/>
-      <c r="G55" s="40"/>
-      <c r="H55" s="40"/>
-      <c r="I55" s="40"/>
-      <c r="J55" s="40"/>
+      <c r="A55" s="42" t="s">
+        <v>55</v>
+      </c>
+      <c r="B55" s="42"/>
+      <c r="C55" s="42"/>
+      <c r="D55" s="42"/>
+      <c r="E55" s="42"/>
+      <c r="F55" s="42"/>
+      <c r="G55" s="42"/>
+      <c r="H55" s="42"/>
+      <c r="I55" s="42"/>
+      <c r="J55" s="42"/>
       <c r="K55" s="16"/>
       <c r="L55" s="16"/>
       <c r="M55" s="16"/>
@@ -3479,18 +3485,18 @@
       <c r="T55" s="16"/>
     </row>
     <row r="56" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="40" t="s">
-        <v>64</v>
-      </c>
-      <c r="B56" s="40"/>
-      <c r="C56" s="40"/>
-      <c r="D56" s="40"/>
-      <c r="E56" s="40"/>
-      <c r="F56" s="40"/>
-      <c r="G56" s="40"/>
-      <c r="H56" s="40"/>
-      <c r="I56" s="40"/>
-      <c r="J56" s="40"/>
+      <c r="A56" s="42" t="s">
+        <v>62</v>
+      </c>
+      <c r="B56" s="42"/>
+      <c r="C56" s="42"/>
+      <c r="D56" s="42"/>
+      <c r="E56" s="42"/>
+      <c r="F56" s="42"/>
+      <c r="G56" s="42"/>
+      <c r="H56" s="42"/>
+      <c r="I56" s="42"/>
+      <c r="J56" s="42"/>
       <c r="K56" s="1"/>
       <c r="L56" s="1"/>
       <c r="M56" s="1"/>
@@ -3554,10 +3560,10 @@
     </row>
     <row r="59" spans="1:20" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A59" s="12" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B59" s="27" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C59" s="1"/>
       <c r="D59" s="1"/>
@@ -3602,7 +3608,7 @@
     </row>
     <row r="61" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A61" s="41" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B61" s="41"/>
       <c r="C61" s="41"/>
@@ -3649,18 +3655,18 @@
       <c r="T62" s="1"/>
     </row>
     <row r="63" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A63" s="40" t="s">
-        <v>59</v>
-      </c>
-      <c r="B63" s="40"/>
-      <c r="C63" s="40"/>
-      <c r="D63" s="40"/>
-      <c r="E63" s="40"/>
-      <c r="F63" s="40"/>
-      <c r="G63" s="40"/>
-      <c r="H63" s="40"/>
-      <c r="I63" s="40"/>
-      <c r="J63" s="40"/>
+      <c r="A63" s="42" t="s">
+        <v>57</v>
+      </c>
+      <c r="B63" s="42"/>
+      <c r="C63" s="42"/>
+      <c r="D63" s="42"/>
+      <c r="E63" s="42"/>
+      <c r="F63" s="42"/>
+      <c r="G63" s="42"/>
+      <c r="H63" s="42"/>
+      <c r="I63" s="42"/>
+      <c r="J63" s="42"/>
       <c r="K63" s="1"/>
       <c r="L63" s="1"/>
       <c r="M63" s="1"/>
@@ -3673,18 +3679,18 @@
       <c r="T63" s="1"/>
     </row>
     <row r="64" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A64" s="40" t="s">
-        <v>60</v>
-      </c>
-      <c r="B64" s="40"/>
-      <c r="C64" s="40"/>
-      <c r="D64" s="40"/>
-      <c r="E64" s="40"/>
-      <c r="F64" s="40"/>
-      <c r="G64" s="40"/>
-      <c r="H64" s="40"/>
-      <c r="I64" s="40"/>
-      <c r="J64" s="40"/>
+      <c r="A64" s="42" t="s">
+        <v>58</v>
+      </c>
+      <c r="B64" s="42"/>
+      <c r="C64" s="42"/>
+      <c r="D64" s="42"/>
+      <c r="E64" s="42"/>
+      <c r="F64" s="42"/>
+      <c r="G64" s="42"/>
+      <c r="H64" s="42"/>
+      <c r="I64" s="42"/>
+      <c r="J64" s="42"/>
       <c r="K64" s="1"/>
       <c r="L64" s="1"/>
       <c r="M64" s="1"/>
@@ -3697,18 +3703,18 @@
       <c r="T64" s="1"/>
     </row>
     <row r="65" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A65" s="40" t="s">
-        <v>73</v>
-      </c>
-      <c r="B65" s="40"/>
-      <c r="C65" s="40"/>
-      <c r="D65" s="40"/>
-      <c r="E65" s="40"/>
-      <c r="F65" s="40"/>
-      <c r="G65" s="40"/>
-      <c r="H65" s="40"/>
-      <c r="I65" s="40"/>
-      <c r="J65" s="40"/>
+      <c r="A65" s="42" t="s">
+        <v>71</v>
+      </c>
+      <c r="B65" s="42"/>
+      <c r="C65" s="42"/>
+      <c r="D65" s="42"/>
+      <c r="E65" s="42"/>
+      <c r="F65" s="42"/>
+      <c r="G65" s="42"/>
+      <c r="H65" s="42"/>
+      <c r="I65" s="42"/>
+      <c r="J65" s="42"/>
       <c r="K65" s="25"/>
       <c r="L65" s="25"/>
       <c r="M65" s="25"/>
@@ -3721,18 +3727,18 @@
       <c r="T65" s="25"/>
     </row>
     <row r="66" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A66" s="40" t="s">
-        <v>72</v>
-      </c>
-      <c r="B66" s="40"/>
-      <c r="C66" s="40"/>
-      <c r="D66" s="40"/>
-      <c r="E66" s="40"/>
-      <c r="F66" s="40"/>
-      <c r="G66" s="40"/>
-      <c r="H66" s="40"/>
-      <c r="I66" s="40"/>
-      <c r="J66" s="40"/>
+      <c r="A66" s="42" t="s">
+        <v>70</v>
+      </c>
+      <c r="B66" s="42"/>
+      <c r="C66" s="42"/>
+      <c r="D66" s="42"/>
+      <c r="E66" s="42"/>
+      <c r="F66" s="42"/>
+      <c r="G66" s="42"/>
+      <c r="H66" s="42"/>
+      <c r="I66" s="42"/>
+      <c r="J66" s="42"/>
       <c r="K66" s="1"/>
       <c r="L66" s="1"/>
       <c r="M66" s="1"/>
@@ -3745,18 +3751,18 @@
       <c r="T66" s="1"/>
     </row>
     <row r="67" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A67" s="40" t="s">
-        <v>81</v>
-      </c>
-      <c r="B67" s="40"/>
-      <c r="C67" s="40"/>
-      <c r="D67" s="40"/>
-      <c r="E67" s="40"/>
-      <c r="F67" s="40"/>
-      <c r="G67" s="40"/>
-      <c r="H67" s="40"/>
-      <c r="I67" s="40"/>
-      <c r="J67" s="40"/>
+      <c r="A67" s="42" t="s">
+        <v>79</v>
+      </c>
+      <c r="B67" s="42"/>
+      <c r="C67" s="42"/>
+      <c r="D67" s="42"/>
+      <c r="E67" s="42"/>
+      <c r="F67" s="42"/>
+      <c r="G67" s="42"/>
+      <c r="H67" s="42"/>
+      <c r="I67" s="42"/>
+      <c r="J67" s="42"/>
       <c r="K67" s="25"/>
       <c r="L67" s="25"/>
       <c r="M67" s="25"/>
@@ -3820,10 +3826,10 @@
     </row>
     <row r="70" spans="1:20" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A70" s="12" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B70" s="13" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C70" s="1"/>
       <c r="D70" s="1"/>
@@ -3868,7 +3874,7 @@
     </row>
     <row r="72" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A72" s="41" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B72" s="41"/>
       <c r="C72" s="41"/>
@@ -3915,18 +3921,18 @@
       <c r="T73" s="1"/>
     </row>
     <row r="74" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A74" s="40" t="s">
-        <v>68</v>
-      </c>
-      <c r="B74" s="40"/>
-      <c r="C74" s="40"/>
-      <c r="D74" s="40"/>
-      <c r="E74" s="40"/>
-      <c r="F74" s="40"/>
-      <c r="G74" s="40"/>
-      <c r="H74" s="40"/>
-      <c r="I74" s="40"/>
-      <c r="J74" s="40"/>
+      <c r="A74" s="42" t="s">
+        <v>66</v>
+      </c>
+      <c r="B74" s="42"/>
+      <c r="C74" s="42"/>
+      <c r="D74" s="42"/>
+      <c r="E74" s="42"/>
+      <c r="F74" s="42"/>
+      <c r="G74" s="42"/>
+      <c r="H74" s="42"/>
+      <c r="I74" s="42"/>
+      <c r="J74" s="42"/>
       <c r="K74" s="1"/>
       <c r="L74" s="1"/>
       <c r="M74" s="1"/>
@@ -3939,18 +3945,18 @@
       <c r="T74" s="1"/>
     </row>
     <row r="75" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A75" s="40" t="s">
-        <v>69</v>
-      </c>
-      <c r="B75" s="40"/>
-      <c r="C75" s="40"/>
-      <c r="D75" s="40"/>
-      <c r="E75" s="40"/>
-      <c r="F75" s="40"/>
-      <c r="G75" s="40"/>
-      <c r="H75" s="40"/>
-      <c r="I75" s="40"/>
-      <c r="J75" s="40"/>
+      <c r="A75" s="42" t="s">
+        <v>67</v>
+      </c>
+      <c r="B75" s="42"/>
+      <c r="C75" s="42"/>
+      <c r="D75" s="42"/>
+      <c r="E75" s="42"/>
+      <c r="F75" s="42"/>
+      <c r="G75" s="42"/>
+      <c r="H75" s="42"/>
+      <c r="I75" s="42"/>
+      <c r="J75" s="42"/>
       <c r="K75" s="19"/>
       <c r="L75" s="19"/>
       <c r="M75" s="19"/>
@@ -3963,18 +3969,18 @@
       <c r="T75" s="19"/>
     </row>
     <row r="76" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A76" s="40" t="s">
-        <v>75</v>
-      </c>
-      <c r="B76" s="40"/>
-      <c r="C76" s="40"/>
-      <c r="D76" s="40"/>
-      <c r="E76" s="40"/>
-      <c r="F76" s="40"/>
-      <c r="G76" s="40"/>
-      <c r="H76" s="40"/>
-      <c r="I76" s="40"/>
-      <c r="J76" s="40"/>
+      <c r="A76" s="42" t="s">
+        <v>73</v>
+      </c>
+      <c r="B76" s="42"/>
+      <c r="C76" s="42"/>
+      <c r="D76" s="42"/>
+      <c r="E76" s="42"/>
+      <c r="F76" s="42"/>
+      <c r="G76" s="42"/>
+      <c r="H76" s="42"/>
+      <c r="I76" s="42"/>
+      <c r="J76" s="42"/>
       <c r="K76" s="25"/>
       <c r="L76" s="25"/>
       <c r="M76" s="25"/>
@@ -3987,18 +3993,18 @@
       <c r="T76" s="25"/>
     </row>
     <row r="77" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A77" s="40" t="s">
-        <v>74</v>
-      </c>
-      <c r="B77" s="40"/>
-      <c r="C77" s="40"/>
-      <c r="D77" s="40"/>
-      <c r="E77" s="40"/>
-      <c r="F77" s="40"/>
-      <c r="G77" s="40"/>
-      <c r="H77" s="40"/>
-      <c r="I77" s="40"/>
-      <c r="J77" s="40"/>
+      <c r="A77" s="42" t="s">
+        <v>72</v>
+      </c>
+      <c r="B77" s="42"/>
+      <c r="C77" s="42"/>
+      <c r="D77" s="42"/>
+      <c r="E77" s="42"/>
+      <c r="F77" s="42"/>
+      <c r="G77" s="42"/>
+      <c r="H77" s="42"/>
+      <c r="I77" s="42"/>
+      <c r="J77" s="42"/>
       <c r="K77" s="25"/>
       <c r="L77" s="25"/>
       <c r="M77" s="25"/>
@@ -4011,18 +4017,18 @@
       <c r="T77" s="25"/>
     </row>
     <row r="78" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A78" s="40" t="s">
-        <v>83</v>
-      </c>
-      <c r="B78" s="40"/>
-      <c r="C78" s="40"/>
-      <c r="D78" s="40"/>
-      <c r="E78" s="40"/>
-      <c r="F78" s="40"/>
-      <c r="G78" s="40"/>
-      <c r="H78" s="40"/>
-      <c r="I78" s="40"/>
-      <c r="J78" s="40"/>
+      <c r="A78" s="42" t="s">
+        <v>81</v>
+      </c>
+      <c r="B78" s="42"/>
+      <c r="C78" s="42"/>
+      <c r="D78" s="42"/>
+      <c r="E78" s="42"/>
+      <c r="F78" s="42"/>
+      <c r="G78" s="42"/>
+      <c r="H78" s="42"/>
+      <c r="I78" s="42"/>
+      <c r="J78" s="42"/>
       <c r="K78" s="1"/>
       <c r="L78" s="1"/>
       <c r="M78" s="1"/>
@@ -4086,10 +4092,10 @@
     </row>
     <row r="81" spans="1:20" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A81" s="12" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B81" s="27" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="C81" s="1"/>
       <c r="D81" s="1"/>
@@ -4134,7 +4140,7 @@
     </row>
     <row r="83" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A83" s="41" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B83" s="41"/>
       <c r="C83" s="41"/>
@@ -4181,18 +4187,18 @@
       <c r="T84" s="1"/>
     </row>
     <row r="85" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A85" s="40" t="s">
-        <v>76</v>
-      </c>
-      <c r="B85" s="40"/>
-      <c r="C85" s="40"/>
-      <c r="D85" s="40"/>
-      <c r="E85" s="40"/>
-      <c r="F85" s="40"/>
-      <c r="G85" s="40"/>
-      <c r="H85" s="40"/>
-      <c r="I85" s="40"/>
-      <c r="J85" s="40"/>
+      <c r="A85" s="42" t="s">
+        <v>74</v>
+      </c>
+      <c r="B85" s="42"/>
+      <c r="C85" s="42"/>
+      <c r="D85" s="42"/>
+      <c r="E85" s="42"/>
+      <c r="F85" s="42"/>
+      <c r="G85" s="42"/>
+      <c r="H85" s="42"/>
+      <c r="I85" s="42"/>
+      <c r="J85" s="42"/>
       <c r="K85" s="1"/>
       <c r="L85" s="1"/>
       <c r="M85" s="1"/>
@@ -4205,18 +4211,18 @@
       <c r="T85" s="1"/>
     </row>
     <row r="86" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A86" s="40" t="s">
-        <v>77</v>
-      </c>
-      <c r="B86" s="40"/>
-      <c r="C86" s="40"/>
-      <c r="D86" s="40"/>
-      <c r="E86" s="40"/>
-      <c r="F86" s="40"/>
-      <c r="G86" s="40"/>
-      <c r="H86" s="40"/>
-      <c r="I86" s="40"/>
-      <c r="J86" s="40"/>
+      <c r="A86" s="42" t="s">
+        <v>75</v>
+      </c>
+      <c r="B86" s="42"/>
+      <c r="C86" s="42"/>
+      <c r="D86" s="42"/>
+      <c r="E86" s="42"/>
+      <c r="F86" s="42"/>
+      <c r="G86" s="42"/>
+      <c r="H86" s="42"/>
+      <c r="I86" s="42"/>
+      <c r="J86" s="42"/>
       <c r="K86" s="25"/>
       <c r="L86" s="25"/>
       <c r="M86" s="25"/>
@@ -4229,18 +4235,18 @@
       <c r="T86" s="25"/>
     </row>
     <row r="87" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A87" s="40" t="s">
-        <v>78</v>
-      </c>
-      <c r="B87" s="40"/>
-      <c r="C87" s="40"/>
-      <c r="D87" s="40"/>
-      <c r="E87" s="40"/>
-      <c r="F87" s="40"/>
-      <c r="G87" s="40"/>
-      <c r="H87" s="40"/>
-      <c r="I87" s="40"/>
-      <c r="J87" s="40"/>
+      <c r="A87" s="42" t="s">
+        <v>76</v>
+      </c>
+      <c r="B87" s="42"/>
+      <c r="C87" s="42"/>
+      <c r="D87" s="42"/>
+      <c r="E87" s="42"/>
+      <c r="F87" s="42"/>
+      <c r="G87" s="42"/>
+      <c r="H87" s="42"/>
+      <c r="I87" s="42"/>
+      <c r="J87" s="42"/>
       <c r="K87" s="25"/>
       <c r="L87" s="25"/>
       <c r="M87" s="25"/>
@@ -4253,18 +4259,18 @@
       <c r="T87" s="25"/>
     </row>
     <row r="88" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A88" s="40" t="s">
-        <v>79</v>
-      </c>
-      <c r="B88" s="40"/>
-      <c r="C88" s="40"/>
-      <c r="D88" s="40"/>
-      <c r="E88" s="40"/>
-      <c r="F88" s="40"/>
-      <c r="G88" s="40"/>
-      <c r="H88" s="40"/>
-      <c r="I88" s="40"/>
-      <c r="J88" s="40"/>
+      <c r="A88" s="42" t="s">
+        <v>77</v>
+      </c>
+      <c r="B88" s="42"/>
+      <c r="C88" s="42"/>
+      <c r="D88" s="42"/>
+      <c r="E88" s="42"/>
+      <c r="F88" s="42"/>
+      <c r="G88" s="42"/>
+      <c r="H88" s="42"/>
+      <c r="I88" s="42"/>
+      <c r="J88" s="42"/>
       <c r="K88" s="1"/>
       <c r="L88" s="1"/>
       <c r="M88" s="1"/>
@@ -4277,18 +4283,18 @@
       <c r="T88" s="1"/>
     </row>
     <row r="89" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A89" s="40" t="s">
-        <v>80</v>
-      </c>
-      <c r="B89" s="40"/>
-      <c r="C89" s="40"/>
-      <c r="D89" s="40"/>
-      <c r="E89" s="40"/>
-      <c r="F89" s="40"/>
-      <c r="G89" s="40"/>
-      <c r="H89" s="40"/>
-      <c r="I89" s="40"/>
-      <c r="J89" s="40"/>
+      <c r="A89" s="42" t="s">
+        <v>78</v>
+      </c>
+      <c r="B89" s="42"/>
+      <c r="C89" s="42"/>
+      <c r="D89" s="42"/>
+      <c r="E89" s="42"/>
+      <c r="F89" s="42"/>
+      <c r="G89" s="42"/>
+      <c r="H89" s="42"/>
+      <c r="I89" s="42"/>
+      <c r="J89" s="42"/>
       <c r="K89" s="25"/>
       <c r="L89" s="25"/>
       <c r="M89" s="25"/>
@@ -4352,10 +4358,10 @@
     </row>
     <row r="92" spans="1:20" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A92" s="12" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B92" s="27" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C92" s="1"/>
       <c r="D92" s="1"/>
@@ -4400,7 +4406,7 @@
     </row>
     <row r="94" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A94" s="41" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B94" s="41"/>
       <c r="C94" s="41"/>
@@ -4447,18 +4453,18 @@
       <c r="T95" s="1"/>
     </row>
     <row r="96" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A96" s="40" t="s">
-        <v>93</v>
-      </c>
-      <c r="B96" s="40"/>
-      <c r="C96" s="40"/>
-      <c r="D96" s="40"/>
-      <c r="E96" s="40"/>
-      <c r="F96" s="40"/>
-      <c r="G96" s="40"/>
-      <c r="H96" s="40"/>
-      <c r="I96" s="40"/>
-      <c r="J96" s="40"/>
+      <c r="A96" s="42" t="s">
+        <v>91</v>
+      </c>
+      <c r="B96" s="42"/>
+      <c r="C96" s="42"/>
+      <c r="D96" s="42"/>
+      <c r="E96" s="42"/>
+      <c r="F96" s="42"/>
+      <c r="G96" s="42"/>
+      <c r="H96" s="42"/>
+      <c r="I96" s="42"/>
+      <c r="J96" s="42"/>
       <c r="K96" s="1"/>
       <c r="L96" s="1"/>
       <c r="M96" s="1"/>
@@ -4471,18 +4477,18 @@
       <c r="T96" s="1"/>
     </row>
     <row r="97" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A97" s="40" t="s">
-        <v>89</v>
-      </c>
-      <c r="B97" s="40"/>
-      <c r="C97" s="40"/>
-      <c r="D97" s="40"/>
-      <c r="E97" s="40"/>
-      <c r="F97" s="40"/>
-      <c r="G97" s="40"/>
-      <c r="H97" s="40"/>
-      <c r="I97" s="40"/>
-      <c r="J97" s="40"/>
+      <c r="A97" s="42" t="s">
+        <v>87</v>
+      </c>
+      <c r="B97" s="42"/>
+      <c r="C97" s="42"/>
+      <c r="D97" s="42"/>
+      <c r="E97" s="42"/>
+      <c r="F97" s="42"/>
+      <c r="G97" s="42"/>
+      <c r="H97" s="42"/>
+      <c r="I97" s="42"/>
+      <c r="J97" s="42"/>
       <c r="K97" s="1"/>
       <c r="L97" s="1"/>
       <c r="M97" s="1"/>
@@ -4495,18 +4501,18 @@
       <c r="T97" s="1"/>
     </row>
     <row r="98" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A98" s="40" t="s">
-        <v>90</v>
-      </c>
-      <c r="B98" s="40"/>
-      <c r="C98" s="40"/>
-      <c r="D98" s="40"/>
-      <c r="E98" s="40"/>
-      <c r="F98" s="40"/>
-      <c r="G98" s="40"/>
-      <c r="H98" s="40"/>
-      <c r="I98" s="40"/>
-      <c r="J98" s="40"/>
+      <c r="A98" s="42" t="s">
+        <v>88</v>
+      </c>
+      <c r="B98" s="42"/>
+      <c r="C98" s="42"/>
+      <c r="D98" s="42"/>
+      <c r="E98" s="42"/>
+      <c r="F98" s="42"/>
+      <c r="G98" s="42"/>
+      <c r="H98" s="42"/>
+      <c r="I98" s="42"/>
+      <c r="J98" s="42"/>
       <c r="K98" s="25"/>
       <c r="L98" s="25"/>
       <c r="M98" s="25"/>
@@ -4519,18 +4525,18 @@
       <c r="T98" s="25"/>
     </row>
     <row r="99" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A99" s="40" t="s">
-        <v>91</v>
-      </c>
-      <c r="B99" s="40"/>
-      <c r="C99" s="40"/>
-      <c r="D99" s="40"/>
-      <c r="E99" s="40"/>
-      <c r="F99" s="40"/>
-      <c r="G99" s="40"/>
-      <c r="H99" s="40"/>
-      <c r="I99" s="40"/>
-      <c r="J99" s="40"/>
+      <c r="A99" s="42" t="s">
+        <v>89</v>
+      </c>
+      <c r="B99" s="42"/>
+      <c r="C99" s="42"/>
+      <c r="D99" s="42"/>
+      <c r="E99" s="42"/>
+      <c r="F99" s="42"/>
+      <c r="G99" s="42"/>
+      <c r="H99" s="42"/>
+      <c r="I99" s="42"/>
+      <c r="J99" s="42"/>
       <c r="K99" s="25"/>
       <c r="L99" s="25"/>
       <c r="M99" s="25"/>
@@ -4543,18 +4549,18 @@
       <c r="T99" s="25"/>
     </row>
     <row r="100" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A100" s="40" t="s">
-        <v>92</v>
-      </c>
-      <c r="B100" s="40"/>
-      <c r="C100" s="40"/>
-      <c r="D100" s="40"/>
-      <c r="E100" s="40"/>
-      <c r="F100" s="40"/>
-      <c r="G100" s="40"/>
-      <c r="H100" s="40"/>
-      <c r="I100" s="40"/>
-      <c r="J100" s="40"/>
+      <c r="A100" s="42" t="s">
+        <v>90</v>
+      </c>
+      <c r="B100" s="42"/>
+      <c r="C100" s="42"/>
+      <c r="D100" s="42"/>
+      <c r="E100" s="42"/>
+      <c r="F100" s="42"/>
+      <c r="G100" s="42"/>
+      <c r="H100" s="42"/>
+      <c r="I100" s="42"/>
+      <c r="J100" s="42"/>
       <c r="K100" s="1"/>
       <c r="L100" s="1"/>
       <c r="M100" s="1"/>
@@ -4567,18 +4573,18 @@
       <c r="T100" s="1"/>
     </row>
     <row r="101" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A101" s="40" t="s">
-        <v>102</v>
-      </c>
-      <c r="B101" s="40"/>
-      <c r="C101" s="40"/>
-      <c r="D101" s="40"/>
-      <c r="E101" s="40"/>
-      <c r="F101" s="40"/>
-      <c r="G101" s="40"/>
-      <c r="H101" s="40"/>
-      <c r="I101" s="40"/>
-      <c r="J101" s="40"/>
+      <c r="A101" s="42" t="s">
+        <v>100</v>
+      </c>
+      <c r="B101" s="42"/>
+      <c r="C101" s="42"/>
+      <c r="D101" s="42"/>
+      <c r="E101" s="42"/>
+      <c r="F101" s="42"/>
+      <c r="G101" s="42"/>
+      <c r="H101" s="42"/>
+      <c r="I101" s="42"/>
+      <c r="J101" s="42"/>
       <c r="K101" s="25"/>
       <c r="L101" s="25"/>
       <c r="M101" s="25"/>
@@ -4642,10 +4648,10 @@
     </row>
     <row r="104" spans="1:20" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A104" s="12" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B104" s="13" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C104" s="1"/>
       <c r="D104" s="1"/>
@@ -4690,7 +4696,7 @@
     </row>
     <row r="106" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A106" s="41" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B106" s="41"/>
       <c r="C106" s="41"/>
@@ -4737,18 +4743,18 @@
       <c r="T107" s="1"/>
     </row>
     <row r="108" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A108" s="40" t="s">
-        <v>97</v>
-      </c>
-      <c r="B108" s="40"/>
-      <c r="C108" s="40"/>
-      <c r="D108" s="40"/>
-      <c r="E108" s="40"/>
-      <c r="F108" s="40"/>
-      <c r="G108" s="40"/>
-      <c r="H108" s="40"/>
-      <c r="I108" s="40"/>
-      <c r="J108" s="40"/>
+      <c r="A108" s="42" t="s">
+        <v>95</v>
+      </c>
+      <c r="B108" s="42"/>
+      <c r="C108" s="42"/>
+      <c r="D108" s="42"/>
+      <c r="E108" s="42"/>
+      <c r="F108" s="42"/>
+      <c r="G108" s="42"/>
+      <c r="H108" s="42"/>
+      <c r="I108" s="42"/>
+      <c r="J108" s="42"/>
       <c r="K108" s="1"/>
       <c r="L108" s="1"/>
       <c r="M108" s="1"/>
@@ -4762,7 +4768,7 @@
     </row>
     <row r="109" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A109" s="1" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B109" s="1"/>
       <c r="C109" s="1"/>
@@ -4785,18 +4791,18 @@
       <c r="T109" s="1"/>
     </row>
     <row r="110" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A110" s="40" t="s">
-        <v>100</v>
-      </c>
-      <c r="B110" s="40"/>
-      <c r="C110" s="40"/>
-      <c r="D110" s="40"/>
-      <c r="E110" s="40"/>
-      <c r="F110" s="40"/>
-      <c r="G110" s="40"/>
-      <c r="H110" s="40"/>
-      <c r="I110" s="40"/>
-      <c r="J110" s="40"/>
+      <c r="A110" s="42" t="s">
+        <v>98</v>
+      </c>
+      <c r="B110" s="42"/>
+      <c r="C110" s="42"/>
+      <c r="D110" s="42"/>
+      <c r="E110" s="42"/>
+      <c r="F110" s="42"/>
+      <c r="G110" s="42"/>
+      <c r="H110" s="42"/>
+      <c r="I110" s="42"/>
+      <c r="J110" s="42"/>
       <c r="K110" s="25"/>
       <c r="L110" s="25"/>
       <c r="M110" s="25"/>
@@ -4809,18 +4815,18 @@
       <c r="T110" s="25"/>
     </row>
     <row r="111" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A111" s="40" t="s">
-        <v>99</v>
-      </c>
-      <c r="B111" s="40"/>
-      <c r="C111" s="40"/>
-      <c r="D111" s="40"/>
-      <c r="E111" s="40"/>
-      <c r="F111" s="40"/>
-      <c r="G111" s="40"/>
-      <c r="H111" s="40"/>
-      <c r="I111" s="40"/>
-      <c r="J111" s="40"/>
+      <c r="A111" s="42" t="s">
+        <v>97</v>
+      </c>
+      <c r="B111" s="42"/>
+      <c r="C111" s="42"/>
+      <c r="D111" s="42"/>
+      <c r="E111" s="42"/>
+      <c r="F111" s="42"/>
+      <c r="G111" s="42"/>
+      <c r="H111" s="42"/>
+      <c r="I111" s="42"/>
+      <c r="J111" s="42"/>
       <c r="K111" s="25"/>
       <c r="L111" s="25"/>
       <c r="M111" s="25"/>
@@ -4833,18 +4839,18 @@
       <c r="T111" s="25"/>
     </row>
     <row r="112" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A112" s="40" t="s">
-        <v>101</v>
-      </c>
-      <c r="B112" s="40"/>
-      <c r="C112" s="40"/>
-      <c r="D112" s="40"/>
-      <c r="E112" s="40"/>
-      <c r="F112" s="40"/>
-      <c r="G112" s="40"/>
-      <c r="H112" s="40"/>
-      <c r="I112" s="40"/>
-      <c r="J112" s="40"/>
+      <c r="A112" s="42" t="s">
+        <v>99</v>
+      </c>
+      <c r="B112" s="42"/>
+      <c r="C112" s="42"/>
+      <c r="D112" s="42"/>
+      <c r="E112" s="42"/>
+      <c r="F112" s="42"/>
+      <c r="G112" s="42"/>
+      <c r="H112" s="42"/>
+      <c r="I112" s="42"/>
+      <c r="J112" s="42"/>
       <c r="K112" s="25"/>
       <c r="L112" s="25"/>
       <c r="M112" s="25"/>
@@ -4908,10 +4914,10 @@
     </row>
     <row r="115" spans="1:20" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A115" s="12" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B115" s="13" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C115" s="1"/>
       <c r="D115" s="1"/>
@@ -4956,7 +4962,7 @@
     </row>
     <row r="117" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A117" s="41" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B117" s="41"/>
       <c r="C117" s="41"/>
@@ -5003,18 +5009,18 @@
       <c r="T118" s="1"/>
     </row>
     <row r="119" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A119" s="40" t="s">
-        <v>108</v>
-      </c>
-      <c r="B119" s="40"/>
-      <c r="C119" s="40"/>
-      <c r="D119" s="40"/>
-      <c r="E119" s="40"/>
-      <c r="F119" s="40"/>
-      <c r="G119" s="40"/>
-      <c r="H119" s="40"/>
-      <c r="I119" s="40"/>
-      <c r="J119" s="40"/>
+      <c r="A119" s="42" t="s">
+        <v>106</v>
+      </c>
+      <c r="B119" s="42"/>
+      <c r="C119" s="42"/>
+      <c r="D119" s="42"/>
+      <c r="E119" s="42"/>
+      <c r="F119" s="42"/>
+      <c r="G119" s="42"/>
+      <c r="H119" s="42"/>
+      <c r="I119" s="42"/>
+      <c r="J119" s="42"/>
       <c r="K119" s="1"/>
       <c r="L119" s="1"/>
       <c r="M119" s="1"/>
@@ -5027,18 +5033,18 @@
       <c r="T119" s="1"/>
     </row>
     <row r="120" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A120" s="40" t="s">
-        <v>109</v>
-      </c>
-      <c r="B120" s="40"/>
-      <c r="C120" s="40"/>
-      <c r="D120" s="40"/>
-      <c r="E120" s="40"/>
-      <c r="F120" s="40"/>
-      <c r="G120" s="40"/>
-      <c r="H120" s="40"/>
-      <c r="I120" s="40"/>
-      <c r="J120" s="40"/>
+      <c r="A120" s="42" t="s">
+        <v>107</v>
+      </c>
+      <c r="B120" s="42"/>
+      <c r="C120" s="42"/>
+      <c r="D120" s="42"/>
+      <c r="E120" s="42"/>
+      <c r="F120" s="42"/>
+      <c r="G120" s="42"/>
+      <c r="H120" s="42"/>
+      <c r="I120" s="42"/>
+      <c r="J120" s="42"/>
       <c r="K120" s="25"/>
       <c r="L120" s="25"/>
       <c r="M120" s="25"/>
@@ -5051,18 +5057,18 @@
       <c r="T120" s="25"/>
     </row>
     <row r="121" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A121" s="40" t="s">
-        <v>110</v>
-      </c>
-      <c r="B121" s="40"/>
-      <c r="C121" s="40"/>
-      <c r="D121" s="40"/>
-      <c r="E121" s="40"/>
-      <c r="F121" s="40"/>
-      <c r="G121" s="40"/>
-      <c r="H121" s="40"/>
-      <c r="I121" s="40"/>
-      <c r="J121" s="40"/>
+      <c r="A121" s="42" t="s">
+        <v>108</v>
+      </c>
+      <c r="B121" s="42"/>
+      <c r="C121" s="42"/>
+      <c r="D121" s="42"/>
+      <c r="E121" s="42"/>
+      <c r="F121" s="42"/>
+      <c r="G121" s="42"/>
+      <c r="H121" s="42"/>
+      <c r="I121" s="42"/>
+      <c r="J121" s="42"/>
       <c r="K121" s="1"/>
       <c r="L121" s="1"/>
       <c r="M121" s="1"/>
@@ -5126,10 +5132,10 @@
     </row>
     <row r="124" spans="1:20" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A124" s="12" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B124" s="27" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C124" s="1"/>
       <c r="D124" s="1"/>
@@ -5174,7 +5180,7 @@
     </row>
     <row r="126" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A126" s="41" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B126" s="41"/>
       <c r="C126" s="41"/>
@@ -5221,18 +5227,18 @@
       <c r="T127" s="1"/>
     </row>
     <row r="128" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A128" s="40" t="s">
-        <v>114</v>
-      </c>
-      <c r="B128" s="40"/>
-      <c r="C128" s="40"/>
-      <c r="D128" s="40"/>
-      <c r="E128" s="40"/>
-      <c r="F128" s="40"/>
-      <c r="G128" s="40"/>
-      <c r="H128" s="40"/>
-      <c r="I128" s="40"/>
-      <c r="J128" s="40"/>
+      <c r="A128" s="42" t="s">
+        <v>112</v>
+      </c>
+      <c r="B128" s="42"/>
+      <c r="C128" s="42"/>
+      <c r="D128" s="42"/>
+      <c r="E128" s="42"/>
+      <c r="F128" s="42"/>
+      <c r="G128" s="42"/>
+      <c r="H128" s="42"/>
+      <c r="I128" s="42"/>
+      <c r="J128" s="42"/>
       <c r="K128" s="1"/>
       <c r="L128" s="1"/>
       <c r="M128" s="1"/>
@@ -5245,18 +5251,18 @@
       <c r="T128" s="1"/>
     </row>
     <row r="129" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A129" s="40" t="s">
-        <v>115</v>
-      </c>
-      <c r="B129" s="40"/>
-      <c r="C129" s="40"/>
-      <c r="D129" s="40"/>
-      <c r="E129" s="40"/>
-      <c r="F129" s="40"/>
-      <c r="G129" s="40"/>
-      <c r="H129" s="40"/>
-      <c r="I129" s="40"/>
-      <c r="J129" s="40"/>
+      <c r="A129" s="42" t="s">
+        <v>113</v>
+      </c>
+      <c r="B129" s="42"/>
+      <c r="C129" s="42"/>
+      <c r="D129" s="42"/>
+      <c r="E129" s="42"/>
+      <c r="F129" s="42"/>
+      <c r="G129" s="42"/>
+      <c r="H129" s="42"/>
+      <c r="I129" s="42"/>
+      <c r="J129" s="42"/>
       <c r="K129" s="25"/>
       <c r="L129" s="25"/>
       <c r="M129" s="25"/>
@@ -5269,18 +5275,18 @@
       <c r="T129" s="25"/>
     </row>
     <row r="130" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A130" s="40" t="s">
-        <v>116</v>
-      </c>
-      <c r="B130" s="40"/>
-      <c r="C130" s="40"/>
-      <c r="D130" s="40"/>
-      <c r="E130" s="40"/>
-      <c r="F130" s="40"/>
-      <c r="G130" s="40"/>
-      <c r="H130" s="40"/>
-      <c r="I130" s="40"/>
-      <c r="J130" s="40"/>
+      <c r="A130" s="42" t="s">
+        <v>114</v>
+      </c>
+      <c r="B130" s="42"/>
+      <c r="C130" s="42"/>
+      <c r="D130" s="42"/>
+      <c r="E130" s="42"/>
+      <c r="F130" s="42"/>
+      <c r="G130" s="42"/>
+      <c r="H130" s="42"/>
+      <c r="I130" s="42"/>
+      <c r="J130" s="42"/>
       <c r="K130" s="1"/>
       <c r="L130" s="1"/>
       <c r="M130" s="1"/>
@@ -5344,10 +5350,10 @@
     </row>
     <row r="133" spans="1:20" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A133" s="12" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B133" s="13" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C133" s="1"/>
       <c r="D133" s="1"/>
@@ -5392,7 +5398,7 @@
     </row>
     <row r="135" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A135" s="41" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B135" s="41"/>
       <c r="C135" s="41"/>
@@ -5439,18 +5445,18 @@
       <c r="T136" s="1"/>
     </row>
     <row r="137" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A137" s="40" t="s">
-        <v>135</v>
-      </c>
-      <c r="B137" s="40"/>
-      <c r="C137" s="40"/>
-      <c r="D137" s="40"/>
-      <c r="E137" s="40"/>
-      <c r="F137" s="40"/>
-      <c r="G137" s="40"/>
-      <c r="H137" s="40"/>
-      <c r="I137" s="40"/>
-      <c r="J137" s="40"/>
+      <c r="A137" s="42" t="s">
+        <v>133</v>
+      </c>
+      <c r="B137" s="42"/>
+      <c r="C137" s="42"/>
+      <c r="D137" s="42"/>
+      <c r="E137" s="42"/>
+      <c r="F137" s="42"/>
+      <c r="G137" s="42"/>
+      <c r="H137" s="42"/>
+      <c r="I137" s="42"/>
+      <c r="J137" s="42"/>
       <c r="K137" s="1"/>
       <c r="L137" s="1"/>
       <c r="M137" s="1"/>
@@ -5463,18 +5469,18 @@
       <c r="T137" s="1"/>
     </row>
     <row r="138" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A138" s="40" t="s">
-        <v>136</v>
-      </c>
-      <c r="B138" s="40"/>
-      <c r="C138" s="40"/>
-      <c r="D138" s="40"/>
-      <c r="E138" s="40"/>
-      <c r="F138" s="40"/>
-      <c r="G138" s="40"/>
-      <c r="H138" s="40"/>
-      <c r="I138" s="40"/>
-      <c r="J138" s="40"/>
+      <c r="A138" s="42" t="s">
+        <v>134</v>
+      </c>
+      <c r="B138" s="42"/>
+      <c r="C138" s="42"/>
+      <c r="D138" s="42"/>
+      <c r="E138" s="42"/>
+      <c r="F138" s="42"/>
+      <c r="G138" s="42"/>
+      <c r="H138" s="42"/>
+      <c r="I138" s="42"/>
+      <c r="J138" s="42"/>
       <c r="K138" s="25"/>
       <c r="L138" s="25"/>
       <c r="M138" s="25"/>
@@ -5487,18 +5493,18 @@
       <c r="T138" s="25"/>
     </row>
     <row r="139" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A139" s="40" t="s">
-        <v>137</v>
-      </c>
-      <c r="B139" s="40"/>
-      <c r="C139" s="40"/>
-      <c r="D139" s="40"/>
-      <c r="E139" s="40"/>
-      <c r="F139" s="40"/>
-      <c r="G139" s="40"/>
-      <c r="H139" s="40"/>
-      <c r="I139" s="40"/>
-      <c r="J139" s="40"/>
+      <c r="A139" s="42" t="s">
+        <v>135</v>
+      </c>
+      <c r="B139" s="42"/>
+      <c r="C139" s="42"/>
+      <c r="D139" s="42"/>
+      <c r="E139" s="42"/>
+      <c r="F139" s="42"/>
+      <c r="G139" s="42"/>
+      <c r="H139" s="42"/>
+      <c r="I139" s="42"/>
+      <c r="J139" s="42"/>
       <c r="K139" s="25"/>
       <c r="L139" s="25"/>
       <c r="M139" s="25"/>
@@ -5562,10 +5568,10 @@
     </row>
     <row r="142" spans="1:20" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A142" s="12" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B142" s="27" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C142" s="1"/>
       <c r="D142" s="1"/>
@@ -5609,18 +5615,18 @@
       <c r="T143" s="1"/>
     </row>
     <row r="144" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A144" s="38" t="s">
-        <v>124</v>
-      </c>
-      <c r="B144" s="38"/>
-      <c r="C144" s="38"/>
-      <c r="D144" s="38"/>
-      <c r="E144" s="38"/>
-      <c r="F144" s="38"/>
-      <c r="G144" s="38"/>
-      <c r="H144" s="38"/>
-      <c r="I144" s="38"/>
-      <c r="J144" s="38"/>
+      <c r="A144" s="46" t="s">
+        <v>122</v>
+      </c>
+      <c r="B144" s="46"/>
+      <c r="C144" s="46"/>
+      <c r="D144" s="46"/>
+      <c r="E144" s="46"/>
+      <c r="F144" s="46"/>
+      <c r="G144" s="46"/>
+      <c r="H144" s="46"/>
+      <c r="I144" s="46"/>
+      <c r="J144" s="46"/>
     </row>
     <row r="145" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A145" s="26" t="s">
@@ -5628,46 +5634,46 @@
       </c>
     </row>
     <row r="146" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A146" s="39" t="s">
+      <c r="A146" s="45" t="s">
+        <v>123</v>
+      </c>
+      <c r="B146" s="45"/>
+      <c r="C146" s="45"/>
+      <c r="D146" s="45"/>
+      <c r="E146" s="45"/>
+      <c r="F146" s="45"/>
+      <c r="G146" s="45"/>
+      <c r="H146" s="45"/>
+      <c r="I146" s="45"/>
+      <c r="J146" s="45"/>
+    </row>
+    <row r="147" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A147" s="45" t="s">
+        <v>124</v>
+      </c>
+      <c r="B147" s="45"/>
+      <c r="C147" s="45"/>
+      <c r="D147" s="45"/>
+      <c r="E147" s="45"/>
+      <c r="F147" s="45"/>
+      <c r="G147" s="45"/>
+      <c r="H147" s="45"/>
+      <c r="I147" s="45"/>
+      <c r="J147" s="45"/>
+    </row>
+    <row r="148" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A148" s="45" t="s">
         <v>125</v>
       </c>
-      <c r="B146" s="39"/>
-      <c r="C146" s="39"/>
-      <c r="D146" s="39"/>
-      <c r="E146" s="39"/>
-      <c r="F146" s="39"/>
-      <c r="G146" s="39"/>
-      <c r="H146" s="39"/>
-      <c r="I146" s="39"/>
-      <c r="J146" s="39"/>
-    </row>
-    <row r="147" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A147" s="39" t="s">
-        <v>126</v>
-      </c>
-      <c r="B147" s="39"/>
-      <c r="C147" s="39"/>
-      <c r="D147" s="39"/>
-      <c r="E147" s="39"/>
-      <c r="F147" s="39"/>
-      <c r="G147" s="39"/>
-      <c r="H147" s="39"/>
-      <c r="I147" s="39"/>
-      <c r="J147" s="39"/>
-    </row>
-    <row r="148" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A148" s="39" t="s">
-        <v>127</v>
-      </c>
-      <c r="B148" s="39"/>
-      <c r="C148" s="39"/>
-      <c r="D148" s="39"/>
-      <c r="E148" s="39"/>
-      <c r="F148" s="39"/>
-      <c r="G148" s="39"/>
-      <c r="H148" s="39"/>
-      <c r="I148" s="39"/>
-      <c r="J148" s="39"/>
+      <c r="B148" s="45"/>
+      <c r="C148" s="45"/>
+      <c r="D148" s="45"/>
+      <c r="E148" s="45"/>
+      <c r="F148" s="45"/>
+      <c r="G148" s="45"/>
+      <c r="H148" s="45"/>
+      <c r="I148" s="45"/>
+      <c r="J148" s="45"/>
     </row>
     <row r="149" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A149" s="11" t="s">
@@ -5685,10 +5691,10 @@
     </row>
     <row r="151" spans="1:10" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A151" s="12" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B151" s="13" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
   </sheetData>
@@ -5703,19 +5709,37 @@
     <mergeCell ref="A129:J129"/>
     <mergeCell ref="A146:J146"/>
     <mergeCell ref="A147:J147"/>
-    <mergeCell ref="A86:J86"/>
-    <mergeCell ref="A87:J87"/>
+    <mergeCell ref="A117:J117"/>
+    <mergeCell ref="A137:J137"/>
+    <mergeCell ref="A138:J138"/>
+    <mergeCell ref="A139:J139"/>
+    <mergeCell ref="A144:J144"/>
     <mergeCell ref="A89:J89"/>
     <mergeCell ref="A67:J67"/>
     <mergeCell ref="A77:J77"/>
-    <mergeCell ref="A98:J98"/>
-    <mergeCell ref="A99:J99"/>
+    <mergeCell ref="A74:J74"/>
+    <mergeCell ref="A78:J78"/>
+    <mergeCell ref="A83:J83"/>
+    <mergeCell ref="A85:J85"/>
+    <mergeCell ref="A75:J75"/>
+    <mergeCell ref="A76:J76"/>
+    <mergeCell ref="A88:J88"/>
     <mergeCell ref="A110:J110"/>
     <mergeCell ref="A29:J29"/>
     <mergeCell ref="A31:J31"/>
     <mergeCell ref="A41:J41"/>
     <mergeCell ref="A42:J42"/>
     <mergeCell ref="A55:J55"/>
+    <mergeCell ref="A30:J30"/>
+    <mergeCell ref="A36:J36"/>
+    <mergeCell ref="A40:J40"/>
+    <mergeCell ref="A43:J43"/>
+    <mergeCell ref="A48:J48"/>
+    <mergeCell ref="A53:J53"/>
+    <mergeCell ref="A54:J54"/>
+    <mergeCell ref="A96:J96"/>
+    <mergeCell ref="A86:J86"/>
+    <mergeCell ref="A87:J87"/>
     <mergeCell ref="A1:R1"/>
     <mergeCell ref="A126:J126"/>
     <mergeCell ref="A128:J128"/>
@@ -5732,37 +5756,19 @@
     <mergeCell ref="A19:J19"/>
     <mergeCell ref="A24:J24"/>
     <mergeCell ref="A28:J28"/>
-    <mergeCell ref="A30:J30"/>
-    <mergeCell ref="A36:J36"/>
-    <mergeCell ref="A40:J40"/>
-    <mergeCell ref="A43:J43"/>
-    <mergeCell ref="A48:J48"/>
-    <mergeCell ref="A53:J53"/>
-    <mergeCell ref="A54:J54"/>
-    <mergeCell ref="A96:J96"/>
     <mergeCell ref="A61:J61"/>
     <mergeCell ref="A63:J63"/>
     <mergeCell ref="A64:J64"/>
     <mergeCell ref="A66:J66"/>
     <mergeCell ref="A72:J72"/>
-    <mergeCell ref="A74:J74"/>
-    <mergeCell ref="A78:J78"/>
-    <mergeCell ref="A83:J83"/>
-    <mergeCell ref="A85:J85"/>
-    <mergeCell ref="A75:J75"/>
     <mergeCell ref="A65:J65"/>
-    <mergeCell ref="A76:J76"/>
-    <mergeCell ref="A88:J88"/>
     <mergeCell ref="A94:J94"/>
     <mergeCell ref="A97:J97"/>
     <mergeCell ref="A100:J100"/>
     <mergeCell ref="A106:J106"/>
     <mergeCell ref="A108:J108"/>
-    <mergeCell ref="A117:J117"/>
-    <mergeCell ref="A137:J137"/>
-    <mergeCell ref="A138:J138"/>
-    <mergeCell ref="A139:J139"/>
-    <mergeCell ref="A144:J144"/>
+    <mergeCell ref="A98:J98"/>
+    <mergeCell ref="A99:J99"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -5771,7 +5777,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:C12"/>
+  <dimension ref="B2:C13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C17" sqref="C17"/>
@@ -5783,80 +5789,88 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C2" s="45" t="s">
-        <v>132</v>
+      <c r="C2" s="29" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="4" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C4" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="5" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C5" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="6" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C6" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="7" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C7" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
     </row>
     <row r="8" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="C8" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
     </row>
     <row r="9" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="C9" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
     </row>
     <row r="10" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C10" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
     </row>
     <row r="11" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="C11" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
     </row>
     <row r="12" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="C12" t="s">
-        <v>156</v>
+        <v>153</v>
+      </c>
+    </row>
+    <row r="13" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>157</v>
+      </c>
+      <c r="C13" t="s">
+        <v>158</v>
       </c>
     </row>
   </sheetData>

</xml_diff>